<commit_message>
Firewall rules added to addressing chart - ',' changed to '.' in IP Address on topology
</commit_message>
<xml_diff>
--- a/Addressing_Table_1.xlsx
+++ b/Addressing_Table_1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forge\OneDrive\Documents\The Final Project\Production-Network---Team-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73437FE2-6745-403F-9A5B-5C6CAD36713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3112B4F8-36A0-4713-AEF5-85FBDE0ADAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
+    <workbookView xWindow="1220" yWindow="410" windowWidth="19610" windowHeight="13910" activeTab="1" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Address Chart" sheetId="2" r:id="rId1"/>
+    <sheet name="Rule Chart" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Device</t>
   </si>
@@ -168,13 +169,124 @@
   </si>
   <si>
     <t>Management Interface</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>Source Zone</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Destination Zone</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Application/Service</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Profiles</t>
+  </si>
+  <si>
+    <t>LAN-to-WAN</t>
+  </si>
+  <si>
+    <t>LAN</t>
+  </si>
+  <si>
+    <t>192.168.150.0/24</t>
+  </si>
+  <si>
+    <t>WAN</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Any (filtered by App-ID/URL filtering)</t>
+  </si>
+  <si>
+    <t>Allow</t>
+  </si>
+  <si>
+    <t>AV, Anti-Spyware, Vulnerability, URL-Filtering</t>
+  </si>
+  <si>
+    <t>LAN-to-DMZ</t>
+  </si>
+  <si>
+    <t>10.17.150.0/24 (specific servers only)</t>
+  </si>
+  <si>
+    <t>Needed Services Only (e.g., LDAP, Syslog)</t>
+  </si>
+  <si>
+    <t>Allow (Restrict)</t>
+  </si>
+  <si>
+    <t>AV, Anti-Spyware, Vulnerability</t>
+  </si>
+  <si>
+    <t>DMZ-to-WAN</t>
+  </si>
+  <si>
+    <t>10.17.150.0/24</t>
+  </si>
+  <si>
+    <t>HTTPS, HTTP (updates only)</t>
+  </si>
+  <si>
+    <t>WAN-to-DMZ</t>
+  </si>
+  <si>
+    <t>Any (Internet)</t>
+  </si>
+  <si>
+    <t>DMZ Public Servers</t>
+  </si>
+  <si>
+    <t>Public Services Only (e.g., HTTPS)</t>
+  </si>
+  <si>
+    <t>WAN-to-LAN</t>
+  </si>
+  <si>
+    <t>Deny</t>
+  </si>
+  <si>
+    <t>Mgmt-Access</t>
+  </si>
+  <si>
+    <t>LAN / Mgmt</t>
+  </si>
+  <si>
+    <t>Trusted Admin IPs</t>
+  </si>
+  <si>
+    <t>Mgmt</t>
+  </si>
+  <si>
+    <t>HTTPS, SSH</t>
+  </si>
+  <si>
+    <t>Allow (restricted)</t>
+  </si>
+  <si>
+    <t>Default-Deny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +316,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,8 +349,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -404,13 +540,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -425,15 +576,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="2" xr:uid="{1CDE1CD4-3DA1-4C8B-921A-BDD02F57EC76}"/>
   </cellStyles>
@@ -769,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EBF2BD-B40B-4074-9942-F9CA6EBDA4C3}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -801,10 +965,10 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -822,10 +986,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -845,10 +1009,10 @@
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
@@ -866,10 +1030,10 @@
       <c r="F5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -889,10 +1053,10 @@
       <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="18"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
@@ -910,10 +1074,10 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="18"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
@@ -931,10 +1095,10 @@
       <c r="F8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="18"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
@@ -952,10 +1116,10 @@
       <c r="F9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
@@ -973,10 +1137,10 @@
       <c r="F10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="18"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
@@ -994,10 +1158,10 @@
       <c r="F11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1017,10 +1181,10 @@
       <c r="F12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1048,4 +1212,497 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20801DFA-768C-44A8-A643-37D6DC24B0F0}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="21"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="21"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="21"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="21"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="21"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="21"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="21"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="21"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="21"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="21"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="21"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="21"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="23"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Firewall rules added to addressing chart - ',' changed to '.' in IP Address on topology"
This reverts commit cf637c39a1b1622586ae7222c262d4ccb3685f1b.
</commit_message>
<xml_diff>
--- a/Addressing_Table_1.xlsx
+++ b/Addressing_Table_1.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forge\OneDrive\Documents\The Final Project\Production-Network---Team-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3112B4F8-36A0-4713-AEF5-85FBDE0ADAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73437FE2-6745-403F-9A5B-5C6CAD36713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="410" windowWidth="19610" windowHeight="13910" activeTab="1" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Address Chart" sheetId="2" r:id="rId1"/>
-    <sheet name="Rule Chart" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Device</t>
   </si>
@@ -169,124 +168,13 @@
   </si>
   <si>
     <t>Management Interface</t>
-  </si>
-  <si>
-    <t>Rule Name</t>
-  </si>
-  <si>
-    <t>Source Zone</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Destination Zone</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>Application/Service</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Profiles</t>
-  </si>
-  <si>
-    <t>LAN-to-WAN</t>
-  </si>
-  <si>
-    <t>LAN</t>
-  </si>
-  <si>
-    <t>192.168.150.0/24</t>
-  </si>
-  <si>
-    <t>WAN</t>
-  </si>
-  <si>
-    <t>Any</t>
-  </si>
-  <si>
-    <t>Any (filtered by App-ID/URL filtering)</t>
-  </si>
-  <si>
-    <t>Allow</t>
-  </si>
-  <si>
-    <t>AV, Anti-Spyware, Vulnerability, URL-Filtering</t>
-  </si>
-  <si>
-    <t>LAN-to-DMZ</t>
-  </si>
-  <si>
-    <t>10.17.150.0/24 (specific servers only)</t>
-  </si>
-  <si>
-    <t>Needed Services Only (e.g., LDAP, Syslog)</t>
-  </si>
-  <si>
-    <t>Allow (Restrict)</t>
-  </si>
-  <si>
-    <t>AV, Anti-Spyware, Vulnerability</t>
-  </si>
-  <si>
-    <t>DMZ-to-WAN</t>
-  </si>
-  <si>
-    <t>10.17.150.0/24</t>
-  </si>
-  <si>
-    <t>HTTPS, HTTP (updates only)</t>
-  </si>
-  <si>
-    <t>WAN-to-DMZ</t>
-  </si>
-  <si>
-    <t>Any (Internet)</t>
-  </si>
-  <si>
-    <t>DMZ Public Servers</t>
-  </si>
-  <si>
-    <t>Public Services Only (e.g., HTTPS)</t>
-  </si>
-  <si>
-    <t>WAN-to-LAN</t>
-  </si>
-  <si>
-    <t>Deny</t>
-  </si>
-  <si>
-    <t>Mgmt-Access</t>
-  </si>
-  <si>
-    <t>LAN / Mgmt</t>
-  </si>
-  <si>
-    <t>Trusted Admin IPs</t>
-  </si>
-  <si>
-    <t>Mgmt</t>
-  </si>
-  <si>
-    <t>HTTPS, SSH</t>
-  </si>
-  <si>
-    <t>Allow (restricted)</t>
-  </si>
-  <si>
-    <t>Default-Deny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,22 +204,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,18 +223,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -540,28 +404,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -576,28 +425,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="2" xr:uid="{1CDE1CD4-3DA1-4C8B-921A-BDD02F57EC76}"/>
   </cellStyles>
@@ -933,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EBF2BD-B40B-4074-9942-F9CA6EBDA4C3}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -965,10 +801,10 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -986,10 +822,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1009,10 +845,10 @@
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
@@ -1030,10 +866,10 @@
       <c r="F5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="18" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1053,10 +889,10 @@
       <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
@@ -1074,10 +910,10 @@
       <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
@@ -1095,10 +931,10 @@
       <c r="F8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="15"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
@@ -1116,10 +952,10 @@
       <c r="F9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="15"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
@@ -1137,10 +973,10 @@
       <c r="F10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="15"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
@@ -1158,10 +994,10 @@
       <c r="F11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="18" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1181,10 +1017,10 @@
       <c r="F12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="16"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1212,497 +1048,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20801DFA-768C-44A8-A643-37D6DC24B0F0}">
-  <dimension ref="A1:H34"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="22"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="22"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="22"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="22"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="22"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="22"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="21"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="22"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="21"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="21"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="21"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="21"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="21"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="21"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="21"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="23"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="24"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
DMZ fixed to come from LAN switch rather than firewall.
</commit_message>
<xml_diff>
--- a/Addressing_Table_1.xlsx
+++ b/Addressing_Table_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forge\Documents\Team7ProjectFolder\Production-Network---Team-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forge\OneDrive\Documents\The Final Project\Production-Network---Team-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C23E6DF-39D6-48A4-A8BD-5F384E7FCD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94FB8C7-F106-428C-A9E7-D198B56B6E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
+    <workbookView xWindow="1220" yWindow="410" windowWidth="19610" windowHeight="13910" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Address Chart" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Device</t>
   </si>
@@ -86,9 +86,6 @@
     <t>E1/2</t>
   </si>
   <si>
-    <t>E1/3</t>
-  </si>
-  <si>
     <t>VLAN1</t>
   </si>
   <si>
@@ -168,6 +165,12 @@
   </si>
   <si>
     <t>Management Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMZ </t>
+  </si>
+  <si>
+    <t>VLAN100</t>
   </si>
 </sst>
 </file>
@@ -767,22 +770,22 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:J15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="7" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -799,247 +802,249 @@
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="16"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addressing Table updated AND Topology ammended to include access for firewall and elastic webapp
</commit_message>
<xml_diff>
--- a/Addressing_Table_1.xlsx
+++ b/Addressing_Table_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forge\OneDrive\Documents\The Final Project\Production-Network---Team-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94FB8C7-F106-428C-A9E7-D198B56B6E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3950B44-8930-4778-87B4-112D3CDB041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="410" windowWidth="19610" windowHeight="13910" xr2:uid="{34E98B91-8496-4094-AC7D-F13B569BAEA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
   <si>
     <t>Device</t>
   </si>
@@ -44,140 +44,173 @@
     <t>Interface</t>
   </si>
   <si>
+    <t>192.168.150.130</t>
+  </si>
+  <si>
+    <t>192.168.150.230</t>
+  </si>
+  <si>
+    <t>192.168.150.50-70</t>
+  </si>
+  <si>
+    <t>192.168.150.20</t>
+  </si>
+  <si>
+    <t>192.168.208.X</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Subnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Gateway </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>E1/2</t>
+  </si>
+  <si>
+    <t>LAN Switch</t>
+  </si>
+  <si>
+    <t>PA Firewall</t>
+  </si>
+  <si>
+    <t>DMZ Server</t>
+  </si>
+  <si>
+    <t>SIEM Server</t>
+  </si>
+  <si>
+    <t>Windows AD Server</t>
+  </si>
+  <si>
+    <t>Windows Client</t>
+  </si>
+  <si>
+    <t>Kali Blue Client</t>
+  </si>
+  <si>
+    <t>Kali Red Client</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>10.17.150.1</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>192.168.150.1</t>
+  </si>
+  <si>
+    <t>PA FIrewall</t>
+  </si>
+  <si>
+    <t>MGMT.</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>DHCP Assigned</t>
+  </si>
+  <si>
+    <t>EXTERNAL</t>
+  </si>
+  <si>
+    <t>192.168.208.1</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>MGMT</t>
+  </si>
+  <si>
+    <t>Inside (LAN)</t>
+  </si>
+  <si>
+    <t>Outside (WAN)</t>
+  </si>
+  <si>
+    <t>DMZ</t>
+  </si>
+  <si>
+    <t>Management Interface</t>
+  </si>
+  <si>
+    <t>VLAN100</t>
+  </si>
+  <si>
+    <t>DMZ Access via LAN Switch</t>
+  </si>
+  <si>
+    <t>E1/8</t>
+  </si>
+  <si>
+    <t>E1/2.150</t>
+  </si>
+  <si>
+    <t>E1/2.200</t>
+  </si>
+  <si>
+    <t>LAN Access &amp; Management</t>
+  </si>
+  <si>
+    <t>VLAN TRUNK</t>
+  </si>
+  <si>
+    <t>10.17.200.1</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>F0/24</t>
+  </si>
+  <si>
+    <t>LAN Ports</t>
+  </si>
+  <si>
+    <t>DMZ Port</t>
+  </si>
+  <si>
+    <t>10.17.200.50</t>
+  </si>
+  <si>
+    <t>192.168.208.28</t>
+  </si>
+  <si>
     <t>192.168.150.254</t>
   </si>
   <si>
-    <t>192.168.150.130</t>
-  </si>
-  <si>
-    <t>192.168.150.230</t>
-  </si>
-  <si>
-    <t>10.17.150.50</t>
-  </si>
-  <si>
-    <t>192.168.150.50-70</t>
-  </si>
-  <si>
-    <t>192.168.150.20</t>
-  </si>
-  <si>
-    <t>192.168.208.X</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Subnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Gateway </t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>E1/1</t>
-  </si>
-  <si>
-    <t>E1/2</t>
-  </si>
-  <si>
-    <t>VLAN1</t>
-  </si>
-  <si>
-    <t>LAN Switch</t>
-  </si>
-  <si>
-    <t>PA Firewall</t>
-  </si>
-  <si>
-    <t>DMZ Server</t>
-  </si>
-  <si>
-    <t>SIEM Server</t>
-  </si>
-  <si>
-    <t>Windows AD Server</t>
-  </si>
-  <si>
-    <t>Windows Client</t>
-  </si>
-  <si>
-    <t>Kali Blue Client</t>
-  </si>
-  <si>
-    <t>Kali Red Client</t>
-  </si>
-  <si>
-    <t>NIC</t>
-  </si>
-  <si>
-    <t>10.17.150.1</t>
-  </si>
-  <si>
-    <t>255.255.255.0</t>
-  </si>
-  <si>
-    <t>192.168.208.1XX</t>
-  </si>
-  <si>
-    <t>255.255.255.255</t>
-  </si>
-  <si>
-    <t>192.168.150.1</t>
-  </si>
-  <si>
-    <t>PA FIrewall</t>
-  </si>
-  <si>
-    <t>MGMT.</t>
-  </si>
-  <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>DHCP Assigned</t>
-  </si>
-  <si>
-    <t>EXTERNAL</t>
-  </si>
-  <si>
-    <t>192.168.208.1</t>
-  </si>
-  <si>
-    <t>Zone</t>
-  </si>
-  <si>
-    <t>MGMT</t>
-  </si>
-  <si>
-    <t>Inside (LAN)</t>
-  </si>
-  <si>
-    <t>Outside (WAN)</t>
-  </si>
-  <si>
-    <t>DMZ</t>
-  </si>
-  <si>
-    <t>Management Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMZ </t>
-  </si>
-  <si>
-    <t>VLAN100</t>
+    <t>VLAN 150/200</t>
+  </si>
+  <si>
+    <t>F0/1-F0/4</t>
+  </si>
+  <si>
+    <t>F0/6-F0/23</t>
+  </si>
+  <si>
+    <t>F0/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +240,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -227,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -400,6 +440,45 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -413,7 +492,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -425,12 +504,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -767,25 +853,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EBF2BD-B40B-4074-9942-F9CA6EBDA4C3}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.81640625" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="7" width="16.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="6" max="8" width="16.81640625" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -793,258 +880,402 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="15">
+        <v>150</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="15">
+        <v>200</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="15">
+        <v>150</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="15">
+        <v>150</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="15">
+        <v>200</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="15">
+        <v>200</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="15">
+        <v>150</v>
+      </c>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="15">
+        <v>150</v>
+      </c>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="15">
+        <v>150</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="16">
+        <v>150</v>
+      </c>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
+      <c r="B19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
+      <c r="C19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="D19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13" t="s">
-        <v>34</v>
+      <c r="E19" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>